<commit_message>
BOM for Rev 3, and design for non-resettable fuses.
</commit_message>
<xml_diff>
--- a/2015/Hardware/BMS_Rev3_Combined_BOM.xlsx
+++ b/2015/Hardware/BMS_Rev3_Combined_BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="22320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28180" windowHeight="22340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="128">
   <si>
     <t>Qty</t>
   </si>
@@ -193,9 +193,6 @@
     <t>Resettable Fuse PTC</t>
   </si>
   <si>
-    <t>RES-11150</t>
-  </si>
-  <si>
     <t>M03POLAR</t>
   </si>
   <si>
@@ -410,19 +407,68 @@
   </si>
   <si>
     <t>SPARKFUN_PN</t>
+  </si>
+  <si>
+    <t>WM4207-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P120FCT-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2N7002WT1GOSCT-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">811-2692-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">445-1423-1-ND </t>
+  </si>
+  <si>
+    <t>490-9967-1-ND</t>
+  </si>
+  <si>
+    <t>NEWARK_PN</t>
+  </si>
+  <si>
+    <t>93B9533</t>
+  </si>
+  <si>
+    <t>Have these already</t>
+  </si>
+  <si>
+    <t>SMD Fuse</t>
+  </si>
+  <si>
+    <t>NON-resettable fuse</t>
+  </si>
+  <si>
+    <t>SF-1206S050-2CT-ND</t>
+  </si>
+  <si>
+    <t>LTC6802IG-2#PBF-ND</t>
+  </si>
+  <si>
+    <t>541-5.1KECT-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -442,13 +488,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -735,15 +785,16 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="6" max="6" width="47.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" customWidth="1"/>
     <col min="8" max="8" width="10.5" customWidth="1"/>
@@ -752,7 +803,7 @@
     <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -772,13 +823,16 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="I1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -795,10 +849,10 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -815,7 +869,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -832,7 +886,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -849,15 +903,15 @@
         <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -872,15 +926,15 @@
         <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
@@ -895,15 +949,15 @@
         <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -917,13 +971,16 @@
       <c r="F8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G8" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -938,10 +995,10 @@
         <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -958,10 +1015,10 @@
         <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -978,10 +1035,10 @@
         <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1001,37 +1058,37 @@
         <v>41</v>
       </c>
       <c r="G12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
         <v>43</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>44</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>45</v>
       </c>
-      <c r="F15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
@@ -1040,13 +1097,13 @@
         <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" t="s">
         <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1054,19 +1111,22 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
         <v>48</v>
-      </c>
-      <c r="C17" t="s">
-        <v>49</v>
       </c>
       <c r="D17">
         <v>1206</v>
       </c>
       <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" t="s">
         <v>50</v>
       </c>
-      <c r="F17" t="s">
-        <v>51</v>
+      <c r="G17" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1074,7 +1134,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -1083,10 +1143,13 @@
         <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F18" t="s">
         <v>29</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1094,28 +1157,31 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" t="s">
         <v>52</v>
       </c>
-      <c r="C19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>53</v>
       </c>
-      <c r="F19" t="s">
-        <v>54</v>
+      <c r="G19" t="s">
+        <v>114</v>
       </c>
       <c r="H19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I19">
         <v>1756827</v>
       </c>
       <c r="J19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1123,22 +1189,25 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
         <v>56</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>57</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>58</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>59</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K20" t="s">
         <v>60</v>
-      </c>
-      <c r="K20" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1146,16 +1215,16 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
         <v>62</v>
       </c>
-      <c r="C21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>63</v>
-      </c>
-      <c r="E21" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1163,7 +1232,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s">
         <v>26</v>
@@ -1172,24 +1241,27 @@
         <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F22" t="s">
         <v>29</v>
       </c>
+      <c r="G22" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" t="s">
-        <v>67</v>
       </c>
       <c r="E23" t="s">
         <v>34</v>
@@ -1200,19 +1272,19 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" t="s">
         <v>68</v>
       </c>
-      <c r="C24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>69</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>70</v>
-      </c>
-      <c r="F24" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -1220,19 +1292,25 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
         <v>72</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>73</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>74</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>75</v>
       </c>
-      <c r="F25" t="s">
-        <v>76</v>
+      <c r="I25" t="s">
+        <v>121</v>
+      </c>
+      <c r="J25" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -1240,19 +1318,19 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" t="s">
         <v>77</v>
       </c>
-      <c r="C26" t="s">
-        <v>77</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>78</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>79</v>
-      </c>
-      <c r="F26" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -1260,16 +1338,16 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" t="s">
         <v>81</v>
       </c>
-      <c r="C27" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>82</v>
-      </c>
-      <c r="E27" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1277,22 +1355,25 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" t="s">
         <v>57</v>
       </c>
-      <c r="C28" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" t="s">
-        <v>58</v>
-      </c>
       <c r="E28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F28" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K28" t="s">
         <v>60</v>
-      </c>
-      <c r="K28" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1300,7 +1381,7 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="C29" t="s">
         <v>38</v>
@@ -1309,13 +1390,13 @@
         <v>39</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F29" t="s">
-        <v>41</v>
-      </c>
-      <c r="K29" t="s">
-        <v>42</v>
+        <v>124</v>
+      </c>
+      <c r="G29" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1323,16 +1404,19 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" t="s">
         <v>86</v>
       </c>
-      <c r="C30" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>87</v>
       </c>
-      <c r="E30" t="s">
-        <v>88</v>
+      <c r="G30" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -1340,19 +1424,22 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" t="s">
         <v>89</v>
       </c>
-      <c r="C31" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>90</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>91</v>
       </c>
-      <c r="F31" t="s">
-        <v>92</v>
+      <c r="G31" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -1360,19 +1447,19 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" t="s">
         <v>93</v>
       </c>
-      <c r="C32" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>94</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>95</v>
-      </c>
-      <c r="F32" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>